<commit_message>
Added new files and added new functions to code
</commit_message>
<xml_diff>
--- a/Ort_Land_Tabelle.xlsx
+++ b/Ort_Land_Tabelle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maurinschucan/Documents/Maurin/Lehre/ZLI/Development_Fundamentals/Project_Happy_Place/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maurinschucan/Documents/Arbeit/Lehre/ZLI/Development_Fundamentals/Project_Happy_Place/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3B0B7A8-E0EA-6241-BA56-8D86EE25860E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EF84ED-7236-F44A-BFC8-B317F5C141A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{6E556217-A9CC-D345-BCEE-F76D1451A9A9}"/>
   </bookViews>

</xml_diff>